<commit_message>
added EMC pre compliance doc number
</commit_message>
<xml_diff>
--- a/GEN-TL-001-01_Document-Reservation-and-Naming-Conventions.xlsx
+++ b/GEN-TL-001-01_Document-Reservation-and-Naming-Conventions.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572AF92-41A3-478D-9CA0-C29BB34B4F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACE6F6F-E509-4619-B72D-71FB7945F30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{4EDE287F-A689-4B21-A551-985357A92207}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4EDE287F-A689-4B21-A551-985357A92207}"/>
   </bookViews>
   <sheets>
     <sheet name="Document No. Convention" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="117">
   <si>
     <t>EE</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>EE-OP-001</t>
+  </si>
+  <si>
+    <t>EE-RD-007</t>
+  </si>
+  <si>
+    <t>EMC Prep &amp; Pre-Compliance</t>
   </si>
 </sst>
 </file>
@@ -1959,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685201DB-FAE9-4A2E-BB07-8EA8C10BA0A0}">
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:B81"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2341,8 +2347,12 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="14"/>
+      <c r="A69" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
@@ -2554,6 +2564,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A101:B101"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A1:B1"/>
@@ -2561,11 +2576,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A101:B101"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B15 B16">
     <cfRule type="expression" dxfId="1" priority="2">

</xml_diff>